<commit_message>
corregir filtrado por TIpo y por Tercio
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\videoanalisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93189EE9-441F-4806-8412-9DBB86E679D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E253D42-2786-43D6-B3EA-8AEE31A947CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,7 +556,18 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:N39" totalsRowShown="0">
-  <autoFilter ref="A1:N39" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
+  <autoFilter ref="A1:N39" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Ataque"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Fase"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -867,7 +878,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -922,7 +933,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1044,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -1074,7 +1085,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +1164,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -1194,7 +1205,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1243,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1281,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1351,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1375,7 +1386,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -1416,7 +1427,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -1454,7 +1465,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1489,7 +1500,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1524,7 +1535,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1559,7 +1570,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1594,7 +1605,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -1673,7 +1684,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>157</v>
       </c>
@@ -1714,7 +1725,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1749,7 +1760,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1787,7 +1798,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +1868,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -1898,7 +1909,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>157</v>
       </c>
@@ -1936,7 +1947,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1974,7 +1985,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2026,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>157</v>
       </c>
@@ -2056,7 +2067,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2105,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2132,7 +2143,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2167,7 +2178,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2205,7 +2216,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2243,7 +2254,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2289,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -2313,7 +2324,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
corregir filtrado por TIpo y por Tercio v2
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\videoanalisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adepa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E253D42-2786-43D6-B3EA-8AEE31A947CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24339A12-64DE-4FBF-9B0C-1B1E76FD3D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,6 +460,9 @@
     <t>Tipo</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=GbtY6G5UVXU</t>
+  </si>
+  <si>
     <t>start_time</t>
   </si>
   <si>
@@ -500,9 +503,6 @@
   </si>
   <si>
     <t>False</t>
-  </si>
-  <si>
-    <t>https://youtu.be/_cq5s5JWDao</t>
   </si>
 </sst>
 </file>
@@ -556,18 +556,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:N39" totalsRowShown="0">
-  <autoFilter ref="A1:N39" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Ataque"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N39" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Fase"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -877,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77939FC4-FC73-4262-977F-310955BE7B1D}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -894,13 +883,13 @@
         <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -930,10 +919,10 @@
         <v>138</v>
       </c>
       <c r="N1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -956,7 +945,7 @@
         <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L2" t="s">
         <v>136</v>
@@ -965,7 +954,7 @@
         <v>139</v>
       </c>
       <c r="N2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -982,7 +971,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -994,7 +983,7 @@
         <v>134</v>
       </c>
       <c r="K3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L3" t="s">
         <v>136</v>
@@ -1003,7 +992,7 @@
         <v>139</v>
       </c>
       <c r="N3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1020,7 +1009,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -1032,7 +1021,7 @@
         <v>134</v>
       </c>
       <c r="K4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L4" t="s">
         <v>136</v>
@@ -1041,12 +1030,12 @@
         <v>139</v>
       </c>
       <c r="N4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1058,7 +1047,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -1073,7 +1062,7 @@
         <v>134</v>
       </c>
       <c r="K5" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L5" t="s">
         <v>136</v>
@@ -1082,10 +1071,10 @@
         <v>139</v>
       </c>
       <c r="N5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1099,7 +1088,7 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -1114,7 +1103,7 @@
         <v>134</v>
       </c>
       <c r="K6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L6" t="s">
         <v>136</v>
@@ -1123,7 +1112,7 @@
         <v>139</v>
       </c>
       <c r="N6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1140,7 +1129,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -1152,7 +1141,7 @@
         <v>134</v>
       </c>
       <c r="K7" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L7" t="s">
         <v>136</v>
@@ -1161,12 +1150,12 @@
         <v>139</v>
       </c>
       <c r="N7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1178,7 +1167,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
         <v>33</v>
@@ -1193,7 +1182,7 @@
         <v>134</v>
       </c>
       <c r="K8" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L8" t="s">
         <v>136</v>
@@ -1202,10 +1191,10 @@
         <v>139</v>
       </c>
       <c r="N8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1219,7 +1208,7 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F9" t="s">
         <v>33</v>
@@ -1231,7 +1220,7 @@
         <v>134</v>
       </c>
       <c r="K9" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L9" t="s">
         <v>136</v>
@@ -1240,10 +1229,10 @@
         <v>139</v>
       </c>
       <c r="N9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1257,7 +1246,7 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -1269,7 +1258,7 @@
         <v>134</v>
       </c>
       <c r="K10" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L10" t="s">
         <v>136</v>
@@ -1278,10 +1267,10 @@
         <v>139</v>
       </c>
       <c r="N10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1293,7 @@
         <v>134</v>
       </c>
       <c r="K11" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L11" t="s">
         <v>137</v>
@@ -1313,10 +1302,10 @@
         <v>139</v>
       </c>
       <c r="N11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1328,7 @@
         <v>134</v>
       </c>
       <c r="K12" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L12" t="s">
         <v>137</v>
@@ -1348,10 +1337,10 @@
         <v>139</v>
       </c>
       <c r="N12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1374,7 +1363,7 @@
         <v>134</v>
       </c>
       <c r="K13" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L13" t="s">
         <v>137</v>
@@ -1383,12 +1372,12 @@
         <v>139</v>
       </c>
       <c r="N13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
@@ -1415,7 +1404,7 @@
         <v>134</v>
       </c>
       <c r="K14" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L14" t="s">
         <v>137</v>
@@ -1424,12 +1413,12 @@
         <v>139</v>
       </c>
       <c r="N14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
@@ -1453,7 +1442,7 @@
         <v>134</v>
       </c>
       <c r="K15" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L15" t="s">
         <v>137</v>
@@ -1462,10 +1451,10 @@
         <v>139</v>
       </c>
       <c r="N15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1477,7 @@
         <v>134</v>
       </c>
       <c r="K16" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L16" t="s">
         <v>137</v>
@@ -1497,10 +1486,10 @@
         <v>139</v>
       </c>
       <c r="N16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1523,7 +1512,7 @@
         <v>134</v>
       </c>
       <c r="K17" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L17" t="s">
         <v>137</v>
@@ -1532,10 +1521,10 @@
         <v>139</v>
       </c>
       <c r="N17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1547,7 @@
         <v>134</v>
       </c>
       <c r="K18" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L18" t="s">
         <v>137</v>
@@ -1567,10 +1556,10 @@
         <v>139</v>
       </c>
       <c r="N18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1593,7 +1582,7 @@
         <v>134</v>
       </c>
       <c r="K19" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L19" t="s">
         <v>137</v>
@@ -1602,10 +1591,10 @@
         <v>139</v>
       </c>
       <c r="N19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1628,7 +1617,7 @@
         <v>134</v>
       </c>
       <c r="K20" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L20" t="s">
         <v>137</v>
@@ -1637,12 +1626,12 @@
         <v>139</v>
       </c>
       <c r="N20" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -1672,7 +1661,7 @@
         <v>134</v>
       </c>
       <c r="K21" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L21" t="s">
         <v>137</v>
@@ -1681,12 +1670,12 @@
         <v>139</v>
       </c>
       <c r="N21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B22" t="s">
         <v>79</v>
@@ -1713,7 +1702,7 @@
         <v>134</v>
       </c>
       <c r="K22" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L22" t="s">
         <v>137</v>
@@ -1722,10 +1711,10 @@
         <v>139</v>
       </c>
       <c r="N22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1737,7 @@
         <v>134</v>
       </c>
       <c r="K23" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L23" t="s">
         <v>137</v>
@@ -1757,10 +1746,10 @@
         <v>139</v>
       </c>
       <c r="N23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1786,7 +1775,7 @@
         <v>134</v>
       </c>
       <c r="K24" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
         <v>137</v>
@@ -1795,12 +1784,12 @@
         <v>139</v>
       </c>
       <c r="N24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
         <v>88</v>
@@ -1821,7 +1810,7 @@
         <v>134</v>
       </c>
       <c r="K25" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L25" t="s">
         <v>137</v>
@@ -1830,10 +1819,10 @@
         <v>139</v>
       </c>
       <c r="N25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +1845,7 @@
         <v>134</v>
       </c>
       <c r="K26" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L26" t="s">
         <v>137</v>
@@ -1865,12 +1854,12 @@
         <v>139</v>
       </c>
       <c r="N26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B27" t="s">
         <v>94</v>
@@ -1897,7 +1886,7 @@
         <v>134</v>
       </c>
       <c r="K27" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L27" t="s">
         <v>137</v>
@@ -1906,12 +1895,12 @@
         <v>139</v>
       </c>
       <c r="N27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
         <v>97</v>
@@ -1935,7 +1924,7 @@
         <v>134</v>
       </c>
       <c r="K28" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L28" t="s">
         <v>137</v>
@@ -1944,10 +1933,10 @@
         <v>139</v>
       </c>
       <c r="N28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1973,7 +1962,7 @@
         <v>134</v>
       </c>
       <c r="K29" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L29" t="s">
         <v>137</v>
@@ -1982,10 +1971,10 @@
         <v>139</v>
       </c>
       <c r="N29" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +2003,7 @@
         <v>134</v>
       </c>
       <c r="K30" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L30" t="s">
         <v>137</v>
@@ -2023,12 +2012,12 @@
         <v>139</v>
       </c>
       <c r="N30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
@@ -2055,7 +2044,7 @@
         <v>134</v>
       </c>
       <c r="K31" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L31" t="s">
         <v>137</v>
@@ -2064,10 +2053,10 @@
         <v>139</v>
       </c>
       <c r="N31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2093,7 +2082,7 @@
         <v>134</v>
       </c>
       <c r="K32" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L32" t="s">
         <v>137</v>
@@ -2102,10 +2091,10 @@
         <v>139</v>
       </c>
       <c r="N32" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2131,7 +2120,7 @@
         <v>134</v>
       </c>
       <c r="K33" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L33" t="s">
         <v>137</v>
@@ -2140,10 +2129,10 @@
         <v>139</v>
       </c>
       <c r="N33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2155,7 @@
         <v>134</v>
       </c>
       <c r="K34" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L34" t="s">
         <v>137</v>
@@ -2175,10 +2164,10 @@
         <v>139</v>
       </c>
       <c r="N34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2204,7 +2193,7 @@
         <v>134</v>
       </c>
       <c r="K35" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L35" t="s">
         <v>137</v>
@@ -2213,10 +2202,10 @@
         <v>139</v>
       </c>
       <c r="N35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2242,7 +2231,7 @@
         <v>134</v>
       </c>
       <c r="K36" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L36" t="s">
         <v>137</v>
@@ -2251,10 +2240,10 @@
         <v>139</v>
       </c>
       <c r="N36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -2277,7 +2266,7 @@
         <v>134</v>
       </c>
       <c r="K37" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L37" t="s">
         <v>137</v>
@@ -2286,10 +2275,10 @@
         <v>139</v>
       </c>
       <c r="N37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -2312,7 +2301,7 @@
         <v>134</v>
       </c>
       <c r="K38" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L38" t="s">
         <v>137</v>
@@ -2321,10 +2310,10 @@
         <v>139</v>
       </c>
       <c r="N38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -2347,7 +2336,7 @@
         <v>134</v>
       </c>
       <c r="K39" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="L39" t="s">
         <v>137</v>
@@ -2356,7 +2345,7 @@
         <v>139</v>
       </c>
       <c r="N39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>